<commit_message>
Update scenario to use 100% CES by 2035 timeline
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/FoPITY/Frac of Pol Impl This Yr - 4 - CA ZEV target.xlsx
+++ b/InputData/plcy-schd/FoPITY/Frac of Pol Impl This Yr - 4 - CA ZEV target.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="6705" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="6705"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -1148,7 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1491,11 +1491,11 @@
   </sheetPr>
   <dimension ref="A1:AI139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F100" sqref="F100"/>
+      <selection pane="bottomRight" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Update scenario to use 100% CES by 2040 timeline
</commit_message>
<xml_diff>
--- a/InputData/plcy-schd/FoPITY/Frac of Pol Impl This Yr - 4 - CA ZEV target.xlsx
+++ b/InputData/plcy-schd/FoPITY/Frac of Pol Impl This Yr - 4 - CA ZEV target.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="6705"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="6705" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -1148,7 +1148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1491,11 +1491,11 @@
   </sheetPr>
   <dimension ref="A1:AI139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C84" sqref="C84"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2189,31 +2189,31 @@
         <v>0</v>
       </c>
       <c r="D19" s="16">
-        <v>0.1016300487881481</v>
+        <v>0.10603488461996206</v>
       </c>
       <c r="E19" s="16">
-        <v>0.20336626727685619</v>
+        <v>0.2124628383905762</v>
       </c>
       <c r="F19" s="16">
-        <v>0.3051295010387125</v>
+        <v>0.31899081006112573</v>
       </c>
       <c r="G19" s="16">
-        <v>0.40697721129800413</v>
+        <v>0.42583153673548502</v>
       </c>
       <c r="H19" s="16">
-        <v>0.49967699348388278</v>
+        <v>0.49880414189421279</v>
       </c>
       <c r="I19" s="16">
-        <v>0.59271654434833276</v>
+        <v>0.57303466324999774</v>
       </c>
       <c r="J19" s="16">
-        <v>0.70346002324921364</v>
+        <v>0.71280994853821689</v>
       </c>
       <c r="K19" s="16">
-        <v>0.80265651305820018</v>
+        <v>0.80983513494432391</v>
       </c>
       <c r="L19" s="16">
-        <v>0.90165009620351222</v>
+        <v>0.90610910561212299</v>
       </c>
       <c r="M19" s="16">
         <v>1</v>
@@ -6935,43 +6935,43 @@
       </c>
       <c r="E10">
         <f>IF(E$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(E$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(E$1,'Set Schedules Here'!18:18,0)),E$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(E$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(E$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(E$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(E$1,'Set Schedules Here'!18:18,1)+1),E$1))</f>
-        <v>0</v>
+        <v>2.8421709430404007E-14</v>
       </c>
       <c r="F10">
         <f>IF(F$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(F$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(F$1,'Set Schedules Here'!18:18,0)),F$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(F$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(F$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(F$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(F$1,'Set Schedules Here'!18:18,1)+1),F$1))</f>
-        <v>0.1016300487881665</v>
+        <v>0.1060348846199588</v>
       </c>
       <c r="G10">
         <f>IF(G$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(G$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(G$1,'Set Schedules Here'!18:18,0)),G$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(G$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(G$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(G$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(G$1,'Set Schedules Here'!18:18,1)+1),G$1))</f>
-        <v>0.2033662672768628</v>
+        <v>0.21246283839059288</v>
       </c>
       <c r="H10">
         <f>IF(H$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(H$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(H$1,'Set Schedules Here'!18:18,0)),H$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(H$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(H$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(H$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(H$1,'Set Schedules Here'!18:18,1)+1),H$1))</f>
-        <v>0.30512950103872072</v>
+        <v>0.31899081006113761</v>
       </c>
       <c r="I10">
         <f>IF(I$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(I$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(I$1,'Set Schedules Here'!18:18,0)),I$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(I$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(I$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(I$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(I$1,'Set Schedules Here'!18:18,1)+1),I$1))</f>
-        <v>0.40697721129799902</v>
+        <v>0.42583153673547258</v>
       </c>
       <c r="J10">
         <f>IF(J$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(J$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(J$1,'Set Schedules Here'!18:18,0)),J$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(J$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(J$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(J$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(J$1,'Set Schedules Here'!18:18,1)+1),J$1))</f>
-        <v>0.49967699348388805</v>
+        <v>0.49880414189422595</v>
       </c>
       <c r="K10">
         <f>IF(K$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(K$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(K$1,'Set Schedules Here'!18:18,0)),K$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(K$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(K$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(K$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(K$1,'Set Schedules Here'!18:18,1)+1),K$1))</f>
-        <v>0.59271654434834886</v>
+        <v>0.57303466324998453</v>
       </c>
       <c r="L10">
         <f>IF(L$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(L$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(L$1,'Set Schedules Here'!18:18,0)),L$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(L$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(L$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(L$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(L$1,'Set Schedules Here'!18:18,1)+1),L$1))</f>
-        <v>0.70346002324919255</v>
+        <v>0.71280994853819379</v>
       </c>
       <c r="M10">
         <f>IF(M$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(M$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(M$1,'Set Schedules Here'!18:18,0)),M$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(M$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(M$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(M$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(M$1,'Set Schedules Here'!18:18,1)+1),M$1))</f>
-        <v>0.80265651305819574</v>
+        <v>0.80983513494430781</v>
       </c>
       <c r="N10">
         <f>IF(N$1=2050,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(N$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(N$1,'Set Schedules Here'!18:18,0)),N$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(N$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(N$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(N$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(N$1,'Set Schedules Here'!18:18,1)+1),N$1))</f>
-        <v>0.90165009620349679</v>
+        <v>0.90610910561210289</v>
       </c>
       <c r="O10">
         <f>IF(O$1=2030,TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(O$1,'Set Schedules Here'!18:18,0)),INDEX('Set Schedules Here'!18:18,1,MATCH(O$1,'Set Schedules Here'!18:18,0)),O$1),TREND(INDEX('Set Schedules Here'!19:19,1,MATCH(O$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!19:19,1,MATCH(O$1,'Set Schedules Here'!18:18,1)+1),INDEX('Set Schedules Here'!18:18,1,MATCH(O$1,'Set Schedules Here'!18:18,1)):INDEX('Set Schedules Here'!18:18,1,MATCH(O$1,'Set Schedules Here'!18:18,1)+1),O$1))</f>
@@ -13112,7 +13112,7 @@
       </c>
       <c r="G10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!D19),"",'Set Schedules Here'!D19)</f>
-        <v>0.1016300487881481</v>
+        <v>0.10603488461996206</v>
       </c>
       <c r="H10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!E18),"",'Set Schedules Here'!E18)</f>
@@ -13120,7 +13120,7 @@
       </c>
       <c r="I10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!E19),"",'Set Schedules Here'!E19)</f>
-        <v>0.20336626727685619</v>
+        <v>0.2124628383905762</v>
       </c>
       <c r="J10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!F18),"",'Set Schedules Here'!F18)</f>
@@ -13128,7 +13128,7 @@
       </c>
       <c r="K10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!F19),"",'Set Schedules Here'!F19)</f>
-        <v>0.3051295010387125</v>
+        <v>0.31899081006112573</v>
       </c>
       <c r="L10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!G18),"",'Set Schedules Here'!G18)</f>
@@ -13136,7 +13136,7 @@
       </c>
       <c r="M10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!G19),"",'Set Schedules Here'!G19)</f>
-        <v>0.40697721129800413</v>
+        <v>0.42583153673548502</v>
       </c>
       <c r="N10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!H18),"",'Set Schedules Here'!H18)</f>
@@ -13144,7 +13144,7 @@
       </c>
       <c r="O10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!H19),"",'Set Schedules Here'!H19)</f>
-        <v>0.49967699348388278</v>
+        <v>0.49880414189421279</v>
       </c>
       <c r="P10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!I18),"",'Set Schedules Here'!I18)</f>
@@ -13152,7 +13152,7 @@
       </c>
       <c r="Q10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!I19),"",'Set Schedules Here'!I19)</f>
-        <v>0.59271654434833276</v>
+        <v>0.57303466324999774</v>
       </c>
       <c r="R10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!J18),"",'Set Schedules Here'!J18)</f>
@@ -13160,7 +13160,7 @@
       </c>
       <c r="S10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!J19),"",'Set Schedules Here'!J19)</f>
-        <v>0.70346002324921364</v>
+        <v>0.71280994853821689</v>
       </c>
       <c r="T10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!K18),"",'Set Schedules Here'!K18)</f>
@@ -13168,7 +13168,7 @@
       </c>
       <c r="U10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!K19),"",'Set Schedules Here'!K19)</f>
-        <v>0.80265651305820018</v>
+        <v>0.80983513494432391</v>
       </c>
       <c r="V10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!L18),"",'Set Schedules Here'!L18)</f>
@@ -13176,7 +13176,7 @@
       </c>
       <c r="W10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!L19),"",'Set Schedules Here'!L19)</f>
-        <v>0.90165009620351222</v>
+        <v>0.90610910561212299</v>
       </c>
       <c r="X10" s="12">
         <f>IF(ISBLANK('Set Schedules Here'!M18),"",'Set Schedules Here'!M18)</f>

</xml_diff>